<commit_message>
from v0.2 to v1.0.1
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar diarias--ART-.xlsx
+++ b/output/xlsx/UC001 - Solicitar diarias--ART-.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Version: </t>
   </si>
   <si>
-    <t>0.1</t>
+    <t>1.0</t>
   </si>
   <si>
     <t>Suite Type:</t>
@@ -230,7 +230,7 @@
     <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
   </si>
   <si>
-    <t>Chefe/Beneficiário Verifica os valores presentes na tela.</t>
+    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado.</t>
   </si>
   <si>
     <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>

</xml_diff>